<commit_message>
Updated Function to compare response body
Updated Function to compare response body
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA0C7516-4A50-4F8C-82E0-B12EF778F9AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB8F049-474C-41F9-A1F5-8DB7B6DC1AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Sl. No. #</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Get User Account with wrong Auth</t>
   </si>
   <si>
-    <t>Verify Team</t>
-  </si>
-  <si>
     <t>GET</t>
   </si>
   <si>
@@ -69,10 +66,19 @@
     <t>ResponseMapValues</t>
   </si>
   <si>
-    <t>account.email_address; account.is_locked</t>
-  </si>
-  <si>
-    <t>aashish.kumar@sofbang.com; false</t>
+    <t>account.email_address;account.is_locked;account.quotas.api_signature_requests_left</t>
+  </si>
+  <si>
+    <t>aashish.kumar@sofbang.com;false;5000</t>
+  </si>
+  <si>
+    <t>Get Team</t>
+  </si>
+  <si>
+    <t>team.name;team.accounts[0].email_address</t>
+  </si>
+  <si>
+    <t>Sofbang Team;vivek.ahuja@sofbang.com</t>
   </si>
 </sst>
 </file>
@@ -420,7 +426,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -451,10 +457,10 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -465,16 +471,20 @@
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>200</v>
       </c>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -484,20 +494,16 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="1">
         <v>200</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -507,10 +513,10 @@
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="1">
         <v>200</v>
@@ -523,23 +529,27 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="D5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="1">
         <v>200</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G3" r:id="rId1" xr:uid="{F43B28CC-7D85-4993-8B4D-5386DCE44FBD}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{A93631B0-72B2-4F8B-86FC-DDB464657E06}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated API validation function
Updated API validation function
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB8F049-474C-41F9-A1F5-8DB7B6DC1AB6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148140F8-11AE-479F-BB69-9682806B68DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -426,7 +426,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated Runner File Only to check an error
Updated Runner File Only to check an error
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3498ED9F-B78D-4A99-B311-E877D1BC6404}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06D1B4E3-596B-481D-8302-BE84CCE3E952}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -75,16 +75,16 @@
     <t>Get Team</t>
   </si>
   <si>
-    <t>team.name;team.accounts[0].email_address</t>
-  </si>
-  <si>
-    <t>Sofbang Team;vivek.ahuja@sofbang.com</t>
-  </si>
-  <si>
     <t>account.email_address</t>
   </si>
   <si>
     <t>aashish.kumar@sofbang.com</t>
+  </si>
+  <si>
+    <t>Sofbang Team;vivek.ahuja@sofbang.com;puneet.gandhi@sofbang.com;5000</t>
+  </si>
+  <si>
+    <t>team.name;team.accounts[0].email_address;team.accounts[1].email_address;team.accounts[1].quotas.api_signature_requests_left</t>
   </si>
 </sst>
 </file>
@@ -432,7 +432,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,8 +442,8 @@
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="79.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -509,10 +509,10 @@
         <v>200</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -551,10 +551,10 @@
         <v>200</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Deposits flow feature file
Added Deposits flow feature file
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAD370F1-A98F-470C-9CC9-95A44D0BA5A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54E6025-8F6D-4278-A5EB-71D0DA6015AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -436,7 +436,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated multiple functions, chat survey and deposits test cases
Updated multiple functions, chat survey and deposits test cases
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F54E6025-8F6D-4278-A5EB-71D0DA6015AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E86F87-7F43-4AF4-938A-B251CFDFC722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -66,12 +66,6 @@
     <t>ResponseMapValues</t>
   </si>
   <si>
-    <t>account.email_address;account.is_locked;account.quotas.api_signature_requests_left</t>
-  </si>
-  <si>
-    <t>aashish.kumar@sofbang.com;false;5000</t>
-  </si>
-  <si>
     <t>Get Team</t>
   </si>
   <si>
@@ -85,6 +79,12 @@
   </si>
   <si>
     <t>team.name;team.accounts[0].account_id;team.accounts[0].email_address;team.accounts[0].is_locked;team.accounts[0].is_paid_hs;team.accounts[0].is_paid_hf;team.accounts[0].quotas.templates_left;team.accounts[0].quotas.documents_left;team.accounts[0].quotas.api_signature_requests_left;team.accounts[0].role_code;team.accounts[1].account_id;team.accounts[1].email_address;team.accounts[1].is_locked;team.accounts[1].is_paid_hs;team.accounts[1].is_paid_hf;team.accounts[1].quotas.templates_left;team.accounts[1].quotas.documents_left;team.accounts[1].quotas.api_signature_requests_left;team.accounts[1].role_code;</t>
+  </si>
+  <si>
+    <t>account.email_address;account.is_locked;account.quotas.api_signature_requests_left;account.quotas.sms_verifications_left</t>
+  </si>
+  <si>
+    <t>aashish.kumar@sofbang.com;false;5000;5000</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,10 +490,10 @@
         <v>200</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -513,10 +513,10 @@
         <v>200</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -543,7 +543,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -555,10 +555,10 @@
         <v>200</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created Emerson API test cases
Created Emerson API test cases
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E86F87-7F43-4AF4-938A-B251CFDFC722}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5793BA73-52EE-4FBC-92CF-70A888E1CDBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>Sl. No. #</t>
   </si>
@@ -85,6 +85,24 @@
   </si>
   <si>
     <t>aashish.kumar@sofbang.com;false;5000;5000</t>
+  </si>
+  <si>
+    <t>Get Login Detail</t>
+  </si>
+  <si>
+    <t>success;data.email;data.ClarityID;data.WorldAreaID;data.city;data.country;data.state;data.zipCode;data.latestAppVersion;data.OFSC_UserID;data.Name;data.Currency</t>
+  </si>
+  <si>
+    <t>true;Aashish.Kumar@Emerson.com;AD_JT_01;12061;Fridabad;IN;Haryana;121007;4.7.1;348;Kumar, Aashish;1</t>
+  </si>
+  <si>
+    <t>Validate user detail</t>
+  </si>
+  <si>
+    <t>success;data.alreadyLoggedIn;data.latestAppVersion</t>
+  </si>
+  <si>
+    <t>true;false;4.7.1</t>
   </si>
 </sst>
 </file>
@@ -144,14 +162,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -433,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -446,8 +469,8 @@
     <col min="3" max="3" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="39" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.140625" customWidth="1"/>
+    <col min="7" max="7" width="46.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -473,7 +496,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -489,10 +512,10 @@
       <c r="E2" s="1">
         <v>200</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
     </row>
@@ -538,7 +561,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -554,11 +577,57 @@
       <c r="E5" s="1">
         <v>200</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="3" t="s">
         <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="1">
+        <v>200</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="1">
+        <v>200</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Emerson API test feature
Emerson API test feature
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FE4CC0B-43CF-42BB-8EDF-91BCE41991E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB153C26-3D83-4EE3-9267-32A66F4513A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
   <si>
     <t>Sl. No. #</t>
   </si>
@@ -117,6 +117,66 @@
   </si>
   <si>
     <t>Emerson</t>
+  </si>
+  <si>
+    <t>Validate Tech Profile for 348</t>
+  </si>
+  <si>
+    <t>success;data.Name;data.OFSC_UserID;data.timeZoneIANA</t>
+  </si>
+  <si>
+    <t>true;Kumar, Aashish;348;Asia/Kolkata</t>
+  </si>
+  <si>
+    <t>Validate Tech Profile for 112</t>
+  </si>
+  <si>
+    <t>true;Faulkner, Richard;112;Europe/London</t>
+  </si>
+  <si>
+    <t>Validate Tech Profile for 343</t>
+  </si>
+  <si>
+    <t>Validate Tech Profile for 34807</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Validate Tech Profile for 000</t>
+  </si>
+  <si>
+    <t>true;Joshi, Khushboo;343;America/Chicago</t>
+  </si>
+  <si>
+    <t>validate user for different udid</t>
+  </si>
+  <si>
+    <t>validate error msg for invalid email</t>
+  </si>
+  <si>
+    <t>validate user with login udid</t>
+  </si>
+  <si>
+    <t>validate user for different email</t>
+  </si>
+  <si>
+    <t>success;data.error.errorCode;data.statusCode</t>
+  </si>
+  <si>
+    <t>true;You are entering wrong email id;422</t>
+  </si>
+  <si>
+    <t>success;data.alreadyLoggedIn</t>
+  </si>
+  <si>
+    <t>true;false</t>
+  </si>
+  <si>
+    <t>true;true</t>
   </si>
 </sst>
 </file>
@@ -189,7 +249,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -204,6 +264,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -486,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,6 +723,213 @@
         <v>24</v>
       </c>
     </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{A93631B0-72B2-4F8B-86FC-DDB464657E06}"/>

</xml_diff>

<commit_message>
Adding all the GET API to git
Adding all the GET API to git
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sohail Abbas\Documents\GitHub\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitData\Sharp\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB153C26-3D83-4EE3-9267-32A66F4513A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95C5CB52-422F-400C-9A22-B28B3413FC90}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="91">
   <si>
     <t>Sl. No. #</t>
   </si>
@@ -177,6 +177,135 @@
   </si>
   <si>
     <t>true;true</t>
+  </si>
+  <si>
+    <t>update UDID</t>
+  </si>
+  <si>
+    <t>update UDID with invalid email</t>
+  </si>
+  <si>
+    <t>update UDID with login</t>
+  </si>
+  <si>
+    <t>success;data.message</t>
+  </si>
+  <si>
+    <t>true;update true</t>
+  </si>
+  <si>
+    <t>success;error.name;error.errorMessage;error.source;error.errorCode;error.httpCode;error.userMessage;context</t>
+  </si>
+  <si>
+    <t>false;errorHandler;User with emailId 'sumit.dahiya@emerson.co' not found;CloudDB;TC-UNKNOWN;404;Resource not setup/active in CloudDB;e5f371db-2c28-4bbe-a2bf-77d2a9519200-0022320e</t>
+  </si>
+  <si>
+    <t>update UDID with logout and invalid email</t>
+  </si>
+  <si>
+    <t>with all valid data</t>
+  </si>
+  <si>
+    <t>success;data.ALLOWANCEID;ALLOWANCETYPE;ORACLEDBID;ENTRYDATE;CREATEDBY;CREATEDDATE;MODIFIEDBY;MODIFIEDDATE;FIELD1;FIELD2;FIELD3;FIELD4;FIELD5;FIELD1_OT;FIELD2_OT;FIELD3_OT;FIELD4_OT;FIELD5_OT;NOTES</t>
+  </si>
+  <si>
+    <t>true;15790082914296056;Overtime;57;2019-10-21;57;14-Jan-2020 01:24:51.429000000 PM;57;14-Jan-2020 01:24:51.429000000 PM;3;1.5;null;null;null;null;null;null;null;null</t>
+  </si>
+  <si>
+    <t>Validate Detailed Notes Attachment for 9</t>
+  </si>
+  <si>
+    <t>Validate Detailed Notes Attachment for 15748581879668350</t>
+  </si>
+  <si>
+    <t>Validate Detailed Notes Attachment for -9</t>
+  </si>
+  <si>
+    <t>Validate Detailed Notes Attachment for 10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Detailed Notes Attachment for </t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>success;data.dnid;data.attachment_id;data.file_name;data.file_type;data.attachment_type;data.modified_by;</t>
+  </si>
+  <si>
+    <t>true;23;9;test.png;png;word file;54</t>
+  </si>
+  <si>
+    <t>true;15748580883511674;15748581879668350;autumn_leaves_PNG3571.png;image/png;DetailedNotes;343</t>
+  </si>
+  <si>
+    <t>Validate FCR Attachment for 1</t>
+  </si>
+  <si>
+    <t>Validate FCR Attachment for -1</t>
+  </si>
+  <si>
+    <t>Validate FCR Attachment for 10</t>
+  </si>
+  <si>
+    <t>Validate FCR Attachment for 15743362115738766</t>
+  </si>
+  <si>
+    <t>success;data.attachment_id;data.attachmenttype;data.file_name;data.task_number;data.attachment_status;data.resourceid;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate FCR Attachment for </t>
+  </si>
+  <si>
+    <t>true;[15743362115738766];[fsr];[Report_15743361053346508_CompletedDebrief-2019-11-21-11-36_en-gb.pdf];[15743361053346508];[true];[1278]</t>
+  </si>
+  <si>
+    <t>true;[1];[1];[2];[1];[1];[1]</t>
+  </si>
+  <si>
+    <t>validate response body for Release Notes</t>
+  </si>
+  <si>
+    <t>true;[1];[1];[1046];</t>
+  </si>
+  <si>
+    <t>success;data.RELEASENOTESID;data.CREATEDBY;data.MODIFIEDBY</t>
+  </si>
+  <si>
+    <t>validate response body for user details</t>
+  </si>
+  <si>
+    <t>success;data.UserID[0];data.Name[0];data.Email[0];data.IsActive[0];data.city[0];data.state[0];data.country[0];data.zipCode[0];data.RoleMappings[0]</t>
+  </si>
+  <si>
+    <t>true;178;Rodney GleN;rodney.glenn@emerson.com;Y;asdada;sadasd;AF;asdsadd;2</t>
+  </si>
+  <si>
+    <t>validate response body for correct user and permission</t>
+  </si>
+  <si>
+    <t>success;data.AMPID[0];data.AppModuleID[0];data.PermissionName[0];data.ModuleName[0];data.URPID[0];</t>
+  </si>
+  <si>
+    <t>true;7;2;ViewLocation;Manage Locations;2159;1</t>
+  </si>
+  <si>
+    <t>validate response body for correct EmergencyCallOut details</t>
+  </si>
+  <si>
+    <t>success;data.Incident_ID[10];data.SR_Number[10];data.Customer_Name[10];data.Project[10];data.Zip_Code[10];data.SR_Group[10];data.SR_Group_ID[10];data.Installed_At_Customer[10]</t>
+  </si>
+  <si>
+    <t>true;1208806;210125-000004;CRISTAL USA INC;ECOMOBILE;70117-4460;CROSSRIDGE;73;TCI INC</t>
+  </si>
+  <si>
+    <t>validate response body for correct role details</t>
+  </si>
+  <si>
+    <t>success;data.UserRoleID[1];data.RoleName[1];data.Description[1]</t>
+  </si>
+  <si>
+    <t>true;15496;Release Manager;Release Notes;</t>
   </si>
 </sst>
 </file>
@@ -249,7 +378,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
@@ -267,6 +396,19 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -549,24 +691,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="67.140625" customWidth="1"/>
-    <col min="7" max="7" width="46.85546875" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.109375" customWidth="1"/>
+    <col min="7" max="7" width="46.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -589,7 +731,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -612,7 +754,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -635,7 +777,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -654,7 +796,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -677,7 +819,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -700,7 +842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -723,7 +865,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -746,7 +888,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -769,7 +911,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -792,7 +934,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -815,7 +957,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -838,7 +980,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -861,7 +1003,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -884,7 +1026,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -907,7 +1049,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -928,6 +1070,487 @@
       </c>
       <c r="G16" s="7" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G21" s="7"/>
+    </row>
+    <row r="22" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="9">
+        <v>31</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="9">
+        <v>32</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A34" s="9">
+        <v>33</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35" s="9">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="9">
+        <v>35</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F36" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G36" s="12" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="9">
+        <v>36</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing SDR API Automation scripts
Committing SDR API Automation scripts
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitData\Sharp\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BA878A-5E7B-4372-B08D-267A24F77F01}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E012F5AE-9D07-426E-9B7F-B0BEB31B3269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="108">
   <si>
     <t>Sl. No. #</t>
   </si>
@@ -312,6 +312,51 @@
   </si>
   <si>
     <t>success;data.Pref_FSR_PrintNote;data.Pref_AddressId;data.Pref_WorldAreaID;data.Pref_ListView</t>
+  </si>
+  <si>
+    <t>validate specific user site data</t>
+  </si>
+  <si>
+    <t>items[1].ID;items[1].VALUE;uris[1];etags[1]</t>
+  </si>
+  <si>
+    <t>12090;Surgut;/mobile/custom/sdranalytics/users/1347/sites/12090;"1f-XDrwCbb23dQiQJkki2qr8wCx73Y"</t>
+  </si>
+  <si>
+    <t>validate reports menu cache</t>
+  </si>
+  <si>
+    <t>items.REPORTID;items.REPORTHEADER_CUSTOMER;items.REPORTHEADER_RONUMBER;items.DEVICEDETAILS_TAG;items.CREATEDBY;uris;etags</t>
+  </si>
+  <si>
+    <t>[dlcIaFJHr9oDyhlEnPxJ9qe5U2W1SOyEfqhT];[change Khushboo];[1234567];[abcdef];[1];[/mobile/custom/sdrmvp/reports/dlcIaFJHr9oDyhlEnPxJ9qe5U2W1SOyEfqhT/menus/dlcIaFJHr9oDyhlEnPxJ9qe5U2W1SOyEfqhT];["338-nehNJQHryyTFs/NJ5wlJ1X1GapU"]</t>
+  </si>
+  <si>
+    <t>validate report devices cache</t>
+  </si>
+  <si>
+    <t>items.REPORTID;items.DEVICETYPE;items.PROCESSTYPE;items.CREATEDBY;uris;etags</t>
+  </si>
+  <si>
+    <t>[dlcIaFJHr9oDyhlEnPxJ9qe5U2W1SOyEfqhT];[1];[340];[1];[/mobile/custom/sdrmvp/reports/dlcIaFJHr9oDyhlEnPxJ9qe5U2W1SOyEfqhT/devices/dlcIaFJHr9oDyhlEnPxJ9qe5U2W1SOyEfqhT];["80-rZanKi3FbEvjfwAHmlLn+xBgmxw"]</t>
+  </si>
+  <si>
+    <t>validate report headers cache</t>
+  </si>
+  <si>
+    <t>items.ID;items.RO_NUMBER;items.FIELD_SERVICE_DIAGNOSTIC_ONLY;items.REPAIR_TYPE;items.REPORT_STATUS;items.EMPLOYEE_NAME;items.CUSTOMER_NAME;items.SERVICE_SITE;uris;etags</t>
+  </si>
+  <si>
+    <t>[dlcIaFJHr9oDyhlEnPxJ9qe5U2W1SOyEfqhT];[1234567];[NO];[Field];[436];[Khushboo J];[change Khushboo];[12096];[/mobile/custom/sdrmvp/reports/dlcIaFJHr9oDyhlEnPxJ9qe5U2W1SOyEfqhT/headers/dlcIaFJHr9oDyhlEnPxJ9qe5U2W1SOyEfqhT];["226-6jVbyEDOOt7uhpitl2LT2S8ezuM"]</t>
+  </si>
+  <si>
+    <t>validate InprogressReports Cache</t>
+  </si>
+  <si>
+    <t>items[1].ID;items[1].RO_NUMBER;items[1].FIELD_SERVICE_DIAGNOSTIC_ONLY;items[1].REPAIR_TYPE;items[1].REPORT_STATUS;items[1].EMPLOYEE_NAME;items[1].CUSTOMER_NAME;items[1].SITE_NAME;uris[1];etags[1]</t>
+  </si>
+  <si>
+    <t>PUWrgePHgrMT2zZxxL6vD5h3mZfBBJfhJ2uu;R3256;NO;Depot;436;Parul Gupta;Khushboo;ABC1;/mobile/custom/sdranalytics/users/1/inprogressreports/PUWrgePHgrMT2zZxxL6vD5h3mZfBBJfhJ2uu;"257-RhuXjhxj6FQctD5qBYVQ0KQ6IEI"</t>
   </si>
 </sst>
 </file>
@@ -700,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1585,6 +1630,121 @@
         <v>86</v>
       </c>
     </row>
+    <row r="39" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" s="9">
+        <v>38</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="G39" s="13" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A40" s="9">
+        <v>39</v>
+      </c>
+      <c r="B40" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="C40" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A41" s="9">
+        <v>40</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C41" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E41" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="G41" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="9">
+        <v>41</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="72" x14ac:dyDescent="0.3">
+      <c r="A43" s="9">
+        <v>42</v>
+      </c>
+      <c r="B43" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E43" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F43" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="G43" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{A93631B0-72B2-4F8B-86FC-DDB464657E06}"/>

</xml_diff>

<commit_message>
Committing Automation code for DEL API
Committing Automation code for 2 DEL SDR APIs
</commit_message>
<xml_diff>
--- a/frameworkDemo/src/test/resources/TestData/TestData.xlsx
+++ b/frameworkDemo/src/test/resources/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitData\Sharp\frameworkDemo1\frameworkDemo\src\test\resources\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E012F5AE-9D07-426E-9B7F-B0BEB31B3269}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD3AC135-DED7-457B-86D8-C71A4568803C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="115">
   <si>
     <t>Sl. No. #</t>
   </si>
@@ -357,6 +357,27 @@
   </si>
   <si>
     <t>PUWrgePHgrMT2zZxxL6vD5h3mZfBBJfhJ2uu;R3256;NO;Depot;436;Parul Gupta;Khushboo;ABC1;/mobile/custom/sdranalytics/users/1/inprogressreports/PUWrgePHgrMT2zZxxL6vD5h3mZfBBJfhJ2uu;"257-RhuXjhxj6FQctD5qBYVQ0KQ6IEI"</t>
+  </si>
+  <si>
+    <t>validate delete user sites</t>
+  </si>
+  <si>
+    <t>DEL</t>
+  </si>
+  <si>
+    <t>status;message</t>
+  </si>
+  <si>
+    <t>200;deactivated successfully</t>
+  </si>
+  <si>
+    <t>validate deactivate report</t>
+  </si>
+  <si>
+    <t>success;data.REPORT_ID;data.Message</t>
+  </si>
+  <si>
+    <t>true;testReport92;Report deactivated successfully.</t>
   </si>
 </sst>
 </file>
@@ -745,10 +766,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G43"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1745,6 +1766,52 @@
         <v>107</v>
       </c>
     </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="9">
+        <v>43</v>
+      </c>
+      <c r="B44" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C44" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E44" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F44" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="G44" s="13" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="9">
+        <v>44</v>
+      </c>
+      <c r="B45" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C45" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F45" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="G45" s="13" t="s">
+        <v>114</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{A93631B0-72B2-4F8B-86FC-DDB464657E06}"/>

</xml_diff>